<commit_message>
Introduction of KP Daily Module
</commit_message>
<xml_diff>
--- a/web/pns/PNS_Daily_Template_20190514_V_4.xlsx
+++ b/web/pns/PNS_Daily_Template_20190514_V_4.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Cohorts\web\pns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7346D495-AC5A-4EA6-9408-3FC9DB94B5DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nd+wG5WmoXHlPB2qPUhqicrnVlfAZlMZvhzuh414fPJaUB1sNM3ltxY56sPEQQ4l+vv9GF/i+PHwP/dW3qzzGA==" workbookSaltValue="lZ0oCjXhczZxW8tnxUVyIg==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BB51A6-E4D6-4111-8981-912A5BC96990}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Zko02fPJVFYj9WIJDZIfVL0HyETKw/HJQUlxl6tOfDrOivZzijZeH1MXZc+ChRESOMGrZXHK5oA/aPnNOsacVg==" workbookSaltValue="Z53STaw+t/SNdXb8vmakVA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <definedName name="Koibatek">'do not delete1'!$Q$1</definedName>
     <definedName name="KoibatekCol">'do not delete1'!$Q$1:$Q$5</definedName>
     <definedName name="KuresoiNorth">'do not delete1'!$R$1</definedName>
-    <definedName name="KuresoiNorthCol">'do not delete1'!$R$1:$R$2</definedName>
+    <definedName name="KuresoiNorthCol">'do not delete1'!$R$1:$R$3</definedName>
     <definedName name="KuresoiSouth">'do not delete1'!$S$1</definedName>
     <definedName name="KuresoiSouthCol">'do not delete1'!$S$1:$S$3</definedName>
     <definedName name="Laikipia">'do not delete1'!$D$1</definedName>
@@ -58,7 +58,7 @@
     <definedName name="LaikipiaNorth">'do not delete1'!$U$1</definedName>
     <definedName name="LaikipiaNorthCol">'do not delete1'!$U$1:$U$3</definedName>
     <definedName name="LaikipiaWest">'do not delete1'!$V$1</definedName>
-    <definedName name="LaikipiaWestCol">'do not delete1'!$V$1:$V$7</definedName>
+    <definedName name="LaikipiaWestCol">'do not delete1'!$V$1:$V$8</definedName>
     <definedName name="Loima">'do not delete1'!$AQ$1</definedName>
     <definedName name="LoimaCol">'do not delete1'!$AQ$1</definedName>
     <definedName name="Loitokitok">'do not delete1'!$X$1</definedName>
@@ -121,13 +121,15 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="89" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -135,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="304">
   <si>
     <t>Total</t>
   </si>
@@ -1197,6 +1199,9 @@
   </si>
   <si>
     <t>St Joseph Nursing home [16409]</t>
+  </si>
+  <si>
+    <t>Maina Village Dispensary [10672]</t>
   </si>
 </sst>
 </file>
@@ -1363,6 +1368,7 @@
       <sz val="10"/>
       <color indexed="0"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1427,7 +1433,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1760,11 +1766,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1908,11 +1923,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1941,30 +1969,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2675,7 +2693,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96EA38A6-102C-4C15-9EF3-CA7FFB8BAABD}" name="PivotTable2" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96EA38A6-102C-4C15-9EF3-CA7FFB8BAABD}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="26">
     <pivotField showAll="0"/>
@@ -3149,8 +3167,8 @@
   </sheetPr>
   <dimension ref="A1:AW39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView showGridLines="0" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3273,7 +3291,7 @@
       <c r="V1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="W1" s="80" t="s">
+      <c r="W1" s="63" t="s">
         <v>301</v>
       </c>
       <c r="X1" s="16" t="s">
@@ -3422,7 +3440,7 @@
       <c r="V2" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="80" t="s">
+      <c r="W2" s="63" t="s">
         <v>77</v>
       </c>
       <c r="X2" s="16" t="s">
@@ -3550,6 +3568,9 @@
       <c r="Q3" s="16" t="s">
         <v>127</v>
       </c>
+      <c r="R3" s="62" t="s">
+        <v>302</v>
+      </c>
       <c r="S3" s="16" t="s">
         <v>152</v>
       </c>
@@ -3562,7 +3583,7 @@
       <c r="V3" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="W3" s="80" t="s">
+      <c r="W3" s="63" t="s">
         <v>299</v>
       </c>
       <c r="X3" s="16" t="s">
@@ -3686,7 +3707,7 @@
       <c r="V4" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="W4" s="80" t="s">
+      <c r="W4" s="63" t="s">
         <v>104</v>
       </c>
       <c r="X4" s="16" t="s">
@@ -3694,9 +3715,6 @@
       </c>
       <c r="Y4" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="AA4" s="79" t="s">
-        <v>302</v>
       </c>
       <c r="AB4" s="16" t="s">
         <v>157</v>
@@ -3800,7 +3818,7 @@
       <c r="V5" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="W5" s="80" t="s">
+      <c r="W5" s="63" t="s">
         <v>131</v>
       </c>
       <c r="X5" s="16" t="s">
@@ -3893,7 +3911,7 @@
       <c r="V6" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="W6" s="80" t="s">
+      <c r="W6" s="63" t="s">
         <v>300</v>
       </c>
       <c r="X6" s="16" t="s">
@@ -3964,7 +3982,7 @@
       <c r="N7" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="V7" s="79" t="s">
+      <c r="V7" s="62" t="s">
         <v>267</v>
       </c>
       <c r="X7" s="16" t="s">
@@ -4006,6 +4024,9 @@
       <c r="K8" s="19"/>
       <c r="L8" s="18"/>
       <c r="M8" s="19"/>
+      <c r="V8" s="82" t="s">
+        <v>303</v>
+      </c>
       <c r="X8" s="16" t="s">
         <v>203</v>
       </c>
@@ -4060,7 +4081,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="18"/>
       <c r="M10" s="19"/>
-      <c r="AB10" s="81" t="s">
+      <c r="AB10" s="64" t="s">
         <v>297</v>
       </c>
       <c r="AE10" s="16" t="s">
@@ -4273,7 +4294,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4w24Mj3O1eHiy4yWtRXZh6KX3znC5A47Eh8QLcZov8GhLl7AJxylf8DS349jpoz2OUBRZjl7WBiVKmNgQTBzng==" saltValue="n0saghMJgWnOlVzpYZ444Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="G2CfvmI3r8czMkIrxjIyCzenx2vLp4TGffKysp1EqwkmDLQnSR7Jefcxv5QTLsdlTHPbIMr9aPKZUSkKd69Hhw==" saltValue="uw2BQ45gRCBpVfAedGFpGg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4290,7 +4311,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4345,64 +4366,64 @@
       <c r="D1" s="58"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="66" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="62" t="s">
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="78" t="s">
+      <c r="M1" s="65"/>
+      <c r="N1" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="78"/>
-      <c r="P1" s="62" t="s">
+      <c r="O1" s="67"/>
+      <c r="P1" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62" t="s">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62" t="s">
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62" t="s">
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62" t="s">
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="78" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4512,7 +4533,7 @@
       <c r="AI2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="63"/>
+      <c r="AJ2" s="78"/>
     </row>
     <row r="3" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
@@ -5177,12 +5198,12 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
@@ -5300,10 +5321,10 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
@@ -5421,10 +5442,10 @@
       </c>
     </row>
     <row r="13" spans="1:36" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
@@ -5691,78 +5712,78 @@
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
       <c r="H16" s="55"/>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="73"/>
-      <c r="AI16" s="73"/>
-      <c r="AJ16" s="73"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="80"/>
+      <c r="AA16" s="80"/>
+      <c r="AB16" s="80"/>
+      <c r="AC16" s="80"/>
+      <c r="AD16" s="80"/>
+      <c r="AE16" s="80"/>
+      <c r="AF16" s="80"/>
+      <c r="AG16" s="80"/>
+      <c r="AH16" s="80"/>
+      <c r="AI16" s="80"/>
+      <c r="AJ16" s="80"/>
     </row>
     <row r="17" spans="1:36" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="68" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76" t="s">
+      <c r="D17" s="68"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="76"/>
-      <c r="AG17" s="76"/>
-      <c r="AH17" s="76"/>
-      <c r="AI17" s="76"/>
-      <c r="AJ17" s="76"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="81"/>
+      <c r="AC17" s="81"/>
+      <c r="AD17" s="81"/>
+      <c r="AE17" s="81"/>
+      <c r="AF17" s="81"/>
+      <c r="AG17" s="81"/>
+      <c r="AH17" s="81"/>
+      <c r="AI17" s="81"/>
+      <c r="AJ17" s="81"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
@@ -5835,8 +5856,10 @@
       <c r="J24" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IcWAMdsUlYMmAUIyjTLJOlA6k7vKEGEOgfYVC34k78LcJZSyDDAD0z2OOaySIRsj0/bzMdBVm8Mo3+lq1e5BHA==" saltValue="Tu+/0wtfHVzL5luzA+7+6A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="biPEfVR8nv3MOmGlNQsBp5F7bqiKb8gzQPTZ6iKOeFA9o9CO4VkwuRW+A6UvHn60LPEWvjwq8AroUQregTjxzw==" saltValue="Cq+IQKiKNNMN5Vmd15SNaQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A11:D13"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="E17:H17"/>
     <mergeCell ref="AH1:AI1"/>
@@ -5855,44 +5878,42 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A11:D13"/>
   </mergeCells>
   <conditionalFormatting sqref="J15:AJ15 J11:AJ13">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AJ11">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:AJ15 J13:AJ13">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:AI7">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5989,64 +6010,64 @@
       <c r="D1" s="58"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="66" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="62" t="s">
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="78" t="s">
+      <c r="M1" s="65"/>
+      <c r="N1" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="78"/>
-      <c r="P1" s="62" t="s">
+      <c r="O1" s="67"/>
+      <c r="P1" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62" t="s">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62" t="s">
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62" t="s">
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62" t="s">
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="78" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6156,7 +6177,7 @@
       <c r="AI2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="63"/>
+      <c r="AJ2" s="78"/>
     </row>
     <row r="3" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
@@ -6821,12 +6842,12 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
@@ -6944,10 +6965,10 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
@@ -7065,10 +7086,10 @@
       </c>
     </row>
     <row r="13" spans="1:36" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
@@ -7335,78 +7356,78 @@
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
       <c r="H16" s="55"/>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="73"/>
-      <c r="AI16" s="73"/>
-      <c r="AJ16" s="73"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="80"/>
+      <c r="AA16" s="80"/>
+      <c r="AB16" s="80"/>
+      <c r="AC16" s="80"/>
+      <c r="AD16" s="80"/>
+      <c r="AE16" s="80"/>
+      <c r="AF16" s="80"/>
+      <c r="AG16" s="80"/>
+      <c r="AH16" s="80"/>
+      <c r="AI16" s="80"/>
+      <c r="AJ16" s="80"/>
     </row>
     <row r="17" spans="1:36" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="68" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76" t="s">
+      <c r="D17" s="68"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="76"/>
-      <c r="AG17" s="76"/>
-      <c r="AH17" s="76"/>
-      <c r="AI17" s="76"/>
-      <c r="AJ17" s="76"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="81"/>
+      <c r="AC17" s="81"/>
+      <c r="AD17" s="81"/>
+      <c r="AE17" s="81"/>
+      <c r="AF17" s="81"/>
+      <c r="AG17" s="81"/>
+      <c r="AH17" s="81"/>
+      <c r="AI17" s="81"/>
+      <c r="AJ17" s="81"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
@@ -7481,62 +7502,62 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="yt7eXD4jiHTOMUN2BDix72s2W0uOyieoXWEitdY+1L4ZZNe3raSSdIdo4IIvfiHb+LuQcn9ZPbBAvcsbPf6uSA==" saltValue="bVd/JFnwBP+onyLurRyuOQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A11:D13"/>
+    <mergeCell ref="I16:AJ16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:AJ17"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="A11:D13"/>
-    <mergeCell ref="I16:AJ16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:AJ17"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="J15:AJ15 J11:AJ13">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AJ11">
-    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:AJ15 J13:AJ13">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:AI7">
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7633,64 +7654,64 @@
       <c r="D1" s="58"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="66" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="62" t="s">
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="78" t="s">
+      <c r="M1" s="65"/>
+      <c r="N1" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="78"/>
-      <c r="P1" s="62" t="s">
+      <c r="O1" s="67"/>
+      <c r="P1" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62" t="s">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62" t="s">
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62" t="s">
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62" t="s">
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="78" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7800,7 +7821,7 @@
       <c r="AI2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="63"/>
+      <c r="AJ2" s="78"/>
     </row>
     <row r="3" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
@@ -8465,12 +8486,12 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
@@ -8588,10 +8609,10 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
@@ -8709,10 +8730,10 @@
       </c>
     </row>
     <row r="13" spans="1:36" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
@@ -8979,78 +9000,78 @@
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
       <c r="H16" s="55"/>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="73"/>
-      <c r="AI16" s="73"/>
-      <c r="AJ16" s="73"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="80"/>
+      <c r="AA16" s="80"/>
+      <c r="AB16" s="80"/>
+      <c r="AC16" s="80"/>
+      <c r="AD16" s="80"/>
+      <c r="AE16" s="80"/>
+      <c r="AF16" s="80"/>
+      <c r="AG16" s="80"/>
+      <c r="AH16" s="80"/>
+      <c r="AI16" s="80"/>
+      <c r="AJ16" s="80"/>
     </row>
     <row r="17" spans="1:36" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="68" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76" t="s">
+      <c r="D17" s="68"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="76"/>
-      <c r="AG17" s="76"/>
-      <c r="AH17" s="76"/>
-      <c r="AI17" s="76"/>
-      <c r="AJ17" s="76"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="81"/>
+      <c r="AC17" s="81"/>
+      <c r="AD17" s="81"/>
+      <c r="AE17" s="81"/>
+      <c r="AF17" s="81"/>
+      <c r="AG17" s="81"/>
+      <c r="AH17" s="81"/>
+      <c r="AI17" s="81"/>
+      <c r="AJ17" s="81"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
@@ -9125,62 +9146,62 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="XTGd5g+zEdJKyL+Ye2hGiYwgZlXGtOUWjONxwyC4GKjaaMOIsGhFzdulLRfie8XqJ82JShxO5lklxKjuILR4JQ==" saltValue="2g5Yf5+ARkc2KT6iyHgOAw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A11:D13"/>
+    <mergeCell ref="I16:AJ16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:AJ17"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="A11:D13"/>
-    <mergeCell ref="I16:AJ16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:AJ17"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="J15:AJ15 J11:AJ13">
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AJ11">
-    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:AJ15 J13:AJ13">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:AI7">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9277,64 +9298,64 @@
       <c r="D1" s="58"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="66" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="62" t="s">
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="78" t="s">
+      <c r="M1" s="65"/>
+      <c r="N1" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="78"/>
-      <c r="P1" s="62" t="s">
+      <c r="O1" s="67"/>
+      <c r="P1" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62" t="s">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62" t="s">
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62" t="s">
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62" t="s">
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="78" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9444,7 +9465,7 @@
       <c r="AI2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="63"/>
+      <c r="AJ2" s="78"/>
     </row>
     <row r="3" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
@@ -10109,12 +10130,12 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
@@ -10232,10 +10253,10 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
@@ -10353,10 +10374,10 @@
       </c>
     </row>
     <row r="13" spans="1:36" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
@@ -10623,78 +10644,78 @@
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
       <c r="H16" s="55"/>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="73"/>
-      <c r="AI16" s="73"/>
-      <c r="AJ16" s="73"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="80"/>
+      <c r="AA16" s="80"/>
+      <c r="AB16" s="80"/>
+      <c r="AC16" s="80"/>
+      <c r="AD16" s="80"/>
+      <c r="AE16" s="80"/>
+      <c r="AF16" s="80"/>
+      <c r="AG16" s="80"/>
+      <c r="AH16" s="80"/>
+      <c r="AI16" s="80"/>
+      <c r="AJ16" s="80"/>
     </row>
     <row r="17" spans="1:36" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="68" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76" t="s">
+      <c r="D17" s="68"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="76"/>
-      <c r="AG17" s="76"/>
-      <c r="AH17" s="76"/>
-      <c r="AI17" s="76"/>
-      <c r="AJ17" s="76"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="81"/>
+      <c r="AC17" s="81"/>
+      <c r="AD17" s="81"/>
+      <c r="AE17" s="81"/>
+      <c r="AF17" s="81"/>
+      <c r="AG17" s="81"/>
+      <c r="AH17" s="81"/>
+      <c r="AI17" s="81"/>
+      <c r="AJ17" s="81"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
@@ -10769,62 +10790,62 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="jonEp2DkkuuMdmW/sTp9BwswAkvrVcWYY3TCpgTrRvTtHmFRJdAhUf8JEOjo6GzgXBV38RGRB/V62gSvaoVlMQ==" saltValue="fjObU97vfornIR9DD1pG4g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A11:D13"/>
+    <mergeCell ref="I16:AJ16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:AJ17"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="A11:D13"/>
-    <mergeCell ref="I16:AJ16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:AJ17"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="J15:AJ15 J11:AJ13">
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AJ11">
-    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:AJ15 J13:AJ13">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:AI7">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10921,64 +10942,64 @@
       <c r="D1" s="58"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="66" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="62" t="s">
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="78" t="s">
+      <c r="M1" s="65"/>
+      <c r="N1" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="78"/>
-      <c r="P1" s="62" t="s">
+      <c r="O1" s="67"/>
+      <c r="P1" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62" t="s">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62" t="s">
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62" t="s">
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62" t="s">
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="78" t="s">
         <v>0</v>
       </c>
     </row>
@@ -11088,7 +11109,7 @@
       <c r="AI2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="63"/>
+      <c r="AJ2" s="78"/>
     </row>
     <row r="3" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
@@ -11753,12 +11774,12 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
@@ -11876,10 +11897,10 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
@@ -11997,10 +12018,10 @@
       </c>
     </row>
     <row r="13" spans="1:36" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
@@ -12267,78 +12288,78 @@
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
       <c r="H16" s="55"/>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="73"/>
-      <c r="AI16" s="73"/>
-      <c r="AJ16" s="73"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="80"/>
+      <c r="AA16" s="80"/>
+      <c r="AB16" s="80"/>
+      <c r="AC16" s="80"/>
+      <c r="AD16" s="80"/>
+      <c r="AE16" s="80"/>
+      <c r="AF16" s="80"/>
+      <c r="AG16" s="80"/>
+      <c r="AH16" s="80"/>
+      <c r="AI16" s="80"/>
+      <c r="AJ16" s="80"/>
     </row>
     <row r="17" spans="1:36" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="68" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76" t="s">
+      <c r="D17" s="68"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="76"/>
-      <c r="AG17" s="76"/>
-      <c r="AH17" s="76"/>
-      <c r="AI17" s="76"/>
-      <c r="AJ17" s="76"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="81"/>
+      <c r="AC17" s="81"/>
+      <c r="AD17" s="81"/>
+      <c r="AE17" s="81"/>
+      <c r="AF17" s="81"/>
+      <c r="AG17" s="81"/>
+      <c r="AH17" s="81"/>
+      <c r="AI17" s="81"/>
+      <c r="AJ17" s="81"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C18" s="12"/>
@@ -12413,6 +12434,9 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Q1hfIFbyJu77en5EqM4mRebZ7fk9BZjeGE4gh7amTenNuPTcDbqVdmRp/Dp7yWJRAIelgTsW1qFOZYM2ZRCCbw==" saltValue="pBLmT0d8/UvsELsibA6FnA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="A11:D13"/>
@@ -12430,45 +12454,42 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="AF1:AG1"/>
   </mergeCells>
   <conditionalFormatting sqref="J15:AJ15 J11:AJ13">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AJ11">
-    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="MFL Code">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="MFL Code">
       <formula>NOT(ISERROR(SEARCH("MFL Code",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:AJ15 J13:AJ13">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:AI7">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:AJ14">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>